<commit_message>
OSP Forms, Contact, Submission Updates
</commit_message>
<xml_diff>
--- a/forms/BudgetProjections1-5YrProject.xlsx
+++ b/forms/BudgetProjections1-5YrProject.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="-90" windowWidth="17325" windowHeight="8580" activeTab="4"/>
+    <workbookView xWindow="2805" yWindow="-90" windowWidth="15360" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="1YearProject" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'4YearProject'!$A$1:$O$203</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'5YearProject'!$A$1:$Q$203</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -477,7 +477,7 @@
     </r>
   </si>
   <si>
-    <t>Fringe Benefits Rate Non-Sponsored and Sponsored 07/01/2014-06/30/2015</t>
+    <t>Fringe Benefits Rate Non-Sponsored and Sponsored 07/01/2015-06/30/2016</t>
   </si>
 </sst>
 </file>
@@ -1309,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1347,7 +1347,7 @@
         <v>99</v>
       </c>
       <c r="K2" s="64">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1358,7 +1358,7 @@
         <v>100</v>
       </c>
       <c r="K3" s="64">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="44">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E9" s="42" t="s">
         <v>52</v>
@@ -1422,7 +1422,7 @@
         <v>51</v>
       </c>
       <c r="C10" s="45">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E10" s="42" t="s">
         <v>0</v>
@@ -1439,7 +1439,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="71">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="J11" s="68" t="s">
         <v>105</v>
@@ -1453,7 +1453,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="45">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="J12" s="68" t="s">
         <v>106</v>
@@ -1508,7 +1508,7 @@
         <v>124</v>
       </c>
       <c r="K16" s="64">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -3235,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M203"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3275,7 +3275,7 @@
         <v>99</v>
       </c>
       <c r="M2" s="64">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -3286,7 +3286,7 @@
         <v>100</v>
       </c>
       <c r="M3" s="64">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="44">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E9" s="42" t="s">
         <v>69</v>
@@ -3354,7 +3354,7 @@
         <v>51</v>
       </c>
       <c r="C10" s="45">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E10" s="42" t="s">
         <v>0</v>
@@ -3371,7 +3371,7 @@
         <v>70</v>
       </c>
       <c r="C11" s="71">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="L11" s="68" t="s">
         <v>105</v>
@@ -3385,7 +3385,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="45">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="L12" s="68" t="s">
         <v>106</v>
@@ -3442,7 +3442,7 @@
         <v>124</v>
       </c>
       <c r="M16" s="64">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -5717,8 +5717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O203"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5782,7 +5782,7 @@
         <v>99</v>
       </c>
       <c r="O2" s="64">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -5805,7 +5805,7 @@
         <v>100</v>
       </c>
       <c r="O3" s="64">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -5917,7 +5917,7 @@
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="44">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="D9" s="42"/>
       <c r="E9" s="42" t="s">
@@ -5944,7 +5944,7 @@
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="45">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42" t="s">
@@ -5971,7 +5971,7 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="71">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="D11" s="42"/>
       <c r="E11" s="42"/>
@@ -5996,7 +5996,7 @@
       </c>
       <c r="B12" s="42"/>
       <c r="C12" s="45">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="D12" s="42"/>
       <c r="E12" s="42"/>
@@ -6100,7 +6100,7 @@
         <v>124</v>
       </c>
       <c r="O16" s="64">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -10489,7 +10489,7 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="F&amp;A Rates" prompt="Select Corresponding Rate" sqref="C13">
-      <formula1>$O$7:$O$21</formula1>
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
@@ -10506,7 +10506,7 @@
   <dimension ref="A1:Q203"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10576,7 +10576,7 @@
         <v>99</v>
       </c>
       <c r="Q2" s="64">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -10601,7 +10601,7 @@
         <v>100</v>
       </c>
       <c r="Q3" s="64">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -10723,7 +10723,7 @@
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="44">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="D9" s="42"/>
       <c r="E9" s="42" t="s">
@@ -10752,7 +10752,7 @@
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="45">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="D10" s="42"/>
       <c r="E10" s="42" t="s">
@@ -10781,7 +10781,7 @@
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="71">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="D11" s="42"/>
       <c r="E11" s="42"/>
@@ -10808,7 +10808,7 @@
       </c>
       <c r="B12" s="42"/>
       <c r="C12" s="45">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="D12" s="42"/>
       <c r="E12" s="42"/>
@@ -10922,7 +10922,7 @@
         <v>124</v>
       </c>
       <c r="Q16" s="64">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -15938,7 +15938,7 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="F&amp;A Rates" prompt="Select Corresponding Rate" sqref="C13">
-      <formula1>$Q$7:$Q$21</formula1>
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
@@ -15956,8 +15956,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16002,7 +16002,7 @@
         <v>99</v>
       </c>
       <c r="S2" s="64">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -16013,7 +16013,7 @@
         <v>100</v>
       </c>
       <c r="S3" s="64">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -16064,7 +16064,7 @@
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="44">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E9" s="42" t="s">
         <v>69</v>
@@ -16081,7 +16081,7 @@
         <v>51</v>
       </c>
       <c r="C10" s="45">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E10" s="42" t="s">
         <v>0</v>
@@ -16098,7 +16098,7 @@
         <v>70</v>
       </c>
       <c r="C11" s="71">
-        <v>0.34300000000000003</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="R11" s="68" t="s">
         <v>105</v>
@@ -16112,7 +16112,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="45">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="R12" s="68" t="s">
         <v>106</v>
@@ -16175,7 +16175,7 @@
         <v>124</v>
       </c>
       <c r="S16" s="64">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
@@ -20439,7 +20439,7 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="F&amp;A Rates" prompt="Select Corresponding Rate" sqref="C13">
-      <formula1>$S$7:$S$21</formula1>
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>